<commit_message>
First Working Version!- VOPS Info HUb app ( New data file structure and permissions)
</commit_message>
<xml_diff>
--- a/Vessel Hazards.xlsx
+++ b/Vessel Hazards.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29010"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F44AD348-26F7-4352-BF74-B7A92C8E336F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F28AB27C-E288-4EE8-AF11-ACE632AD7CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>Vessel Name</t>
   </si>
@@ -56,6 +56,9 @@
     <t>Risk Assessment Document Link</t>
   </si>
   <si>
+    <t>Vessel Info Link</t>
+  </si>
+  <si>
     <t>Sea Cruiser 2</t>
   </si>
   <si>
@@ -71,6 +74,9 @@
     <t xml:space="preserve">same again </t>
   </si>
   <si>
+    <t>https://www.marinetraffic.com/en/ais/details/ships/shipid:665124/mmsi:355104000/imo:9196319/vessel:SEA_CRUISER_2</t>
+  </si>
+  <si>
     <t>EMS Highway</t>
   </si>
   <si>
@@ -83,6 +89,9 @@
     <t>https://risk-assesment.pdf</t>
   </si>
   <si>
+    <t>https://www.marinetraffic.com/en/ais/details/ships/shipid:146379/mmsi:212882000/imo:9195133/vessel:EMS_HIGHWAY</t>
+  </si>
+  <si>
     <t>Thames Highway</t>
   </si>
   <si>
@@ -92,10 +101,16 @@
     <t>http://shi[pdecks.com/Thames.pdf</t>
   </si>
   <si>
+    <t>https://www.marinetraffic.com/en/ais/details/ships/shipid:376403/mmsi:311996000/imo:9316294/vessel:THAMES_HIGHWAY</t>
+  </si>
+  <si>
     <t>Vessel</t>
   </si>
   <si>
-    <t>Deck Number</t>
+    <t>Deck Id</t>
+  </si>
+  <si>
+    <t>Deck</t>
   </si>
   <si>
     <t>Average Deck Height (m)</t>
@@ -132,6 +147,15 @@
   </si>
   <si>
     <t>FIxed</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B01</t>
+  </si>
+  <si>
+    <t>WD</t>
   </si>
   <si>
     <t>Comment Title</t>
@@ -315,9 +339,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDB4AD42-9875-410D-94E9-26C99453DC8D}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:G4" xr:uid="{CDB4AD42-9875-410D-94E9-26C99453DC8D}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDB4AD42-9875-410D-94E9-26C99453DC8D}" name="Table1" displayName="Table1" ref="A1:H4" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:H4" xr:uid="{CDB4AD42-9875-410D-94E9-26C99453DC8D}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0EFB4FE3-2198-4765-BCFE-36EE1C5C3C21}" name="Vessel Name"/>
     <tableColumn id="2" xr3:uid="{CB1F3938-532E-4641-BEA3-67E0D0B06FC9}" name="Capacity"/>
     <tableColumn id="9" xr3:uid="{192A328B-32BF-4EB5-9D62-16D908FDBDC9}" name="Number of Decks"/>
@@ -325,17 +349,19 @@
     <tableColumn id="12" xr3:uid="{71A7B901-AEDE-42A9-B6CC-06BD38C5CD4F}" name="Additional Hazards"/>
     <tableColumn id="10" xr3:uid="{A594E2F7-A675-45F8-8C27-1516B512D142}" name="Deck Layout Link"/>
     <tableColumn id="11" xr3:uid="{A4B689BA-270B-4210-9D64-C1EAEA8E66E1}" name="Risk Assessment Document Link" dataCellStyle="Hyperlink"/>
+    <tableColumn id="3" xr3:uid="{23F5FC1D-0064-4313-84D6-87DB742D76AC}" name="Vessel Info Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2C485FB5-543A-4C28-8E82-6911C7AEB740}" name="Table4" displayName="Table4" ref="A1:E25" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:E25" xr:uid="{2C485FB5-543A-4C28-8E82-6911C7AEB740}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2C485FB5-543A-4C28-8E82-6911C7AEB740}" name="Table4" displayName="Table4" ref="A1:F25" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:F25" xr:uid="{2C485FB5-543A-4C28-8E82-6911C7AEB740}"/>
+  <tableColumns count="6">
     <tableColumn id="2" xr3:uid="{0AD038C4-0BB6-475A-8473-C32D9D40448B}" name="Vessel"/>
-    <tableColumn id="3" xr3:uid="{63363FFD-EF7C-4D6B-A771-2C87109477A3}" name="Deck Number"/>
+    <tableColumn id="1" xr3:uid="{8F19A802-1ECF-42A3-84C9-BA87B68032BE}" name="Deck Id"/>
+    <tableColumn id="3" xr3:uid="{63363FFD-EF7C-4D6B-A771-2C87109477A3}" name="Deck"/>
     <tableColumn id="4" xr3:uid="{97B50412-D051-4634-893D-6D05243CA0EB}" name="Average Deck Height (m)"/>
     <tableColumn id="5" xr3:uid="{7F076D0E-6B66-473D-A102-E21116691EFB}" name="Deck Type"/>
     <tableColumn id="6" xr3:uid="{5D6F3648-9464-4751-A3EA-2D52C210CB1B}" name="Notes"/>
@@ -675,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -690,9 +716,10 @@
     <col min="5" max="5" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="110.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1">
+    <row r="1" spans="1:8" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -714,10 +741,13 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>802</v>
@@ -726,21 +756,24 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>876</v>
@@ -749,18 +782,21 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>2000</v>
@@ -769,13 +805,16 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>15</v>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -785,400 +824,479 @@
     <hyperlink ref="G3" r:id="rId3" xr:uid="{228A5937-63E9-493B-8561-350B132C7558}"/>
     <hyperlink ref="F4" r:id="rId4" xr:uid="{5D0FC1A2-244D-40BB-873F-D7DABF61985E}"/>
     <hyperlink ref="G4" r:id="rId5" xr:uid="{A2848E92-E999-4345-B987-84FA0FE748A1}"/>
+    <hyperlink ref="H2" r:id="rId6" xr:uid="{AC91CAB9-C7C6-4220-92F9-69404828A7F9}"/>
+    <hyperlink ref="H3" r:id="rId7" xr:uid="{945CE4E3-7631-43E2-8F8B-6023ED039E0C}"/>
+    <hyperlink ref="H4" r:id="rId8" xr:uid="{7ACD75F8-7603-43A6-8E65-7FDC22B767CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8826B921-D234-41C5-9356-DF31C962DAEF}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
       <c r="E2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>30</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3">
         <v>2.4</v>
       </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4">
         <v>2.5</v>
       </c>
-      <c r="D4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6">
+        <v>2.8</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="C6">
-        <v>2.8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
         <v>2.4</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>4</v>
       </c>
       <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>5</v>
       </c>
       <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
         <v>2.4</v>
       </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>6</v>
       </c>
       <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12">
         <v>2.4</v>
       </c>
-      <c r="D12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>7</v>
       </c>
       <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13">
         <v>2.4</v>
       </c>
-      <c r="D13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
       <c r="E14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15">
         <v>2.4</v>
       </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
       <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
         <v>2.4</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
         <v>2.4</v>
       </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="E17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>5</v>
       </c>
       <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18">
         <v>2.4</v>
       </c>
-      <c r="D18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>6</v>
       </c>
       <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
         <v>2.4</v>
       </c>
-      <c r="D19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>7</v>
       </c>
       <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
         <v>2.4</v>
       </c>
-      <c r="D20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>8</v>
       </c>
       <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
         <v>2.4</v>
       </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B22">
         <v>9</v>
       </c>
       <c r="C22">
+        <v>9</v>
+      </c>
+      <c r="D22">
         <v>2.4</v>
       </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B23">
         <v>10</v>
       </c>
       <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
-        <v>25</v>
-      </c>
       <c r="E23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>30</v>
+      </c>
+      <c r="F23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>11</v>
       </c>
       <c r="C24">
+        <v>11</v>
+      </c>
+      <c r="D24">
         <v>2</v>
       </c>
-      <c r="D24" t="s">
-        <v>32</v>
-      </c>
       <c r="E24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>12</v>
       </c>
-      <c r="C25">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25">
         <v>2</v>
       </c>
-      <c r="D25" t="s">
-        <v>25</v>
-      </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1194,7 +1312,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1208,87 +1326,87 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C2" s="5">
         <v>45817</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C3" s="5">
         <v>45819</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5">
         <v>45820</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5">
         <v>45826</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>